<commit_message>
did 2 questions only
</commit_message>
<xml_diff>
--- a/450 questions.xlsx
+++ b/450 questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bablove/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashyc7\Desktop\Data-Structures-and-Algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254D2BE7-30E0-4BA9-84C2-FAF9BE26F08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="16200" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="3765" yWindow="4800" windowWidth="15375" windowHeight="7875" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1426,6 +1426,9 @@
   </si>
   <si>
     <t xml:space="preserve">Youtube Channel: https://www.youtube.com/channel/UCQHLxxBFrbfdrk1jF0moTpw </t>
+  </si>
+  <si>
+    <t>&lt;Yes&gt;</t>
   </si>
 </sst>
 </file>
@@ -1857,18 +1860,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="123" customWidth="1"/>
+    <col min="2" max="2" width="104.375" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26">
+    <row r="1" spans="1:3" ht="26.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1891,7 +1894,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="C5" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21">
@@ -1902,7 +1905,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21">

</xml_diff>